<commit_message>
Excel sheet writer finalised
</commit_message>
<xml_diff>
--- a/data/cold_email_data.xlsx
+++ b/data/cold_email_data.xlsx
@@ -8,38 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\portfolio projects\ColdFlow\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A70B4B-222B-4DF6-BAB4-068369D3E865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737DE2F4-0ACA-4E0D-BAF2-1D7E26157556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+  <si>
+    <t>Company_Name</t>
+  </si>
   <si>
     <t>Email_Recipient</t>
   </si>
   <si>
-    <t>Company_Name</t>
-  </si>
-  <si>
     <t>Email_id</t>
   </si>
   <si>
@@ -58,7 +46,7 @@
     <t>Prompt</t>
   </si>
   <si>
-    <t>Email_content</t>
+    <t>Content</t>
   </si>
   <si>
     <t>Status</t>
@@ -73,6 +61,33 @@
     <t>n.b24fnmail@gmail.com</t>
   </si>
   <si>
+    <t>2025-03-30</t>
+  </si>
+  <si>
+    <t>For the position of waiter at Cattleman's Ranch</t>
+  </si>
+  <si>
+    <t>[Your Name]
+[Your Address]
+[City, State, ZIP]
+[Date]
+[Hiring Manager's Name]
+Cattleman's Ranch
+[Ranch Address]
+[City, State, ZIP]
+Dear [Hiring Manager's Name],
+I am excited to apply for the Waiter position at Cattleman's Ranch, where I can utilize my exceptional customer service skills and passion for delivering outstanding dining experiences. With a strong foundation in hospitality and a keen interest in providing top-notch service, I am confident that I would make a valuable addition to your team.
+As a highly motivated and energetic individual, I possess excellent communication and interpersonal skills, which enable me to build strong relationships with customers, colleagues, and management. My previous experience in the food service industry has taught me the importance of attention to detail, multitasking, and working well under pressure. I am confident that my skills and experience make me an ideal candidate for this role.
+I am particularly drawn to Cattleman's Ranch because of its reputation for providing high-quality food and exceptional customer service in a unique and rustic setting. I am impressed by the ranch's commitment to using only the freshest ingredients and its dedication to creating a warm and welcoming atmosphere for guests. I am excited about the opportunity to be a part of a team that shares my passion for delivering exceptional customer experiences.
+In addition to my technical skills and experience, I possess a strong work ethic and a willingness to learn and adapt to new situations. I am available to work a variety of shifts, including weekends and holidays, and I am committed to providing outstanding service to every guest, every time.
+Thank you for considering my application. I would be thrilled to discuss this opportunity further and explain in greater detail why I am the ideal candidate for this role. Please do not hesitate to contact me at [Your Phone Number] or [Your Email Address].
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t>Email Sent.</t>
+  </si>
+  <si>
     <t>TupperWare</t>
   </si>
   <si>
@@ -82,10 +97,26 @@
     <t>badwaiknakul@gmail.com</t>
   </si>
   <si>
-    <t>For the position of waiter at Cattleman's Ranch</t>
-  </si>
-  <si>
     <t>For the position of salesman at TupperWare</t>
+  </si>
+  <si>
+    <t>[Your Name]
+[Your Address]
+[City, State, ZIP]
+[Date]
+[Hiring Manager's Name]
+TupperWare
+[TupperWare's Address]
+[City, State, ZIP]
+Dear [Hiring Manager's Name],
+I am excited to apply for the Salesman position at TupperWare, a renowned brand that has been a household name for decades. With a passion for building relationships and driving sales growth, I am confident that my skills and experience make me an ideal fit for this role.
+As a highly motivated and results-driven sales professional, I have a proven track record of consistently meeting and exceeding sales targets. My excellent communication and interpersonal skills enable me to effectively engage with customers, understand their needs, and provide tailored solutions that meet their expectations. I am well-versed in product knowledge and have a keen ability to demonstrate the benefits and features of TupperWare's innovative products.
+I am particularly drawn to TupperWare's commitment to providing high-quality, durable, and functional products that make a positive impact on people's lives. I am impressed by the company's dedication to empowering individuals, especially women, through its business opportunities and community involvement. As someone who values integrity, teamwork, and customer satisfaction, I am excited about the opportunity to join an organization that shares these values.
+In my current role at [Current Company], I have gained valuable experience in sales, customer service, and team management. I have successfully developed and executed sales strategies, built strong relationships with customers, and consistently achieved sales targets. I am confident that my skills and experience will enable me to make a significant contribution to TupperWare's sales team.
+I am excited about the opportunity to work with TupperWare's iconic products and to be part of a team that is dedicated to making a positive impact on people's lives. I am confident that my passion, energy, and sales expertise make me an ideal candidate for this role. I would welcome the opportunity to discuss my application and how I can contribute to TupperWare's success.
+Thank you for considering my application. I look forward to the opportunity to meet with you to discuss this role further.
+Sincerely,
+[Your Name]</t>
   </si>
 </sst>
 </file>
@@ -163,15 +194,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -181,6 +209,15 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -487,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +539,7 @@
     <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="10" max="10" width="62.28515625" customWidth="1"/>
+    <col min="10" max="10" width="83.5703125" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -510,94 +547,106 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:11" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3</v>
+      </c>
+      <c r="G3" s="4">
+        <v>45746</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="171" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2">
         <v>5</v>
       </c>
-      <c r="F3" s="3">
-        <v>3</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="4">
         <v>45746</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3">
-        <v>5</v>
-      </c>
-      <c r="F4" s="3">
-        <v>2</v>
-      </c>
-      <c r="G4" s="5">
-        <v>45747</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{8544B1B0-803A-4ACB-AEE8-E04CA8A5B6EB}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{0EECA571-A533-4AAF-80BE-B39BE84C4049}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
ui changes and logo added
</commit_message>
<xml_diff>
--- a/data/cold_email_data.xlsx
+++ b/data/cold_email_data.xlsx
@@ -478,10 +478,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -494,9 +494,9 @@
     <col width="14.42578125" bestFit="1" customWidth="1" min="6" max="6"/>
     <col width="22.5703125" bestFit="1" customWidth="1" min="7" max="7"/>
     <col width="22" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="25.42578125" customWidth="1" min="9" max="9"/>
-    <col width="83.5703125" customWidth="1" min="10" max="10"/>
-    <col width="15.7109375" customWidth="1" min="11" max="11"/>
+    <col width="25.42578125" customWidth="1" min="9" max="10"/>
+    <col width="83.5703125" customWidth="1" min="11" max="11"/>
+    <col width="15.7109375" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -546,10 +546,15 @@
       </c>
       <c r="J2" s="5" t="inlineStr">
         <is>
+          <t>Subject</t>
+        </is>
+      </c>
+      <c r="K2" s="5" t="inlineStr">
+        <is>
           <t>Content</t>
         </is>
       </c>
-      <c r="K2" s="5" t="inlineStr">
+      <c r="L2" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
@@ -587,30 +592,21 @@
       </c>
       <c r="I3" s="7" t="inlineStr">
         <is>
-          <t>For the position of waiter at Cattleman's Ranch</t>
+          <t>Write an cover letter for sending and email to Cattleman's Ranch's Manager, Mr Loius Huang. I want to work as a waiter there. Make it short and concise, just 2 paragraphs. My name is Nakul and 20 years old. No need to add subject line and NO PREAMBLE!</t>
         </is>
       </c>
       <c r="J3" s="7" t="inlineStr">
         <is>
-          <t>[Your Name]
-[Your Address]
-[City, State, ZIP]
-[Date]
-[Hiring Manager's Name]
-Cattleman's Ranch
-[Ranch Address]
-[City, State, ZIP]
-Dear [Hiring Manager's Name],
-I am excited to apply for the Waiter position at Cattleman's Ranch, where I can utilize my exceptional customer service skills and passion for delivering outstanding dining experiences. With a strong foundation in hospitality and a keen interest in providing top-notch service, I am confident that I would make a valuable addition to your team.
-As a highly motivated and energetic individual, I possess excellent communication and interpersonal skills, which enable me to build strong relationships with customers, colleagues, and management. My previous experience in the food service industry has taught me the importance of attention to detail, multitasking, and working well under pressure. I am confident that my skills and experience make me an ideal candidate for this role.
-I am particularly drawn to Cattleman's Ranch because of its reputation for providing high-quality food and exceptional customer service in a unique and rustic setting. I am impressed by the ranch's commitment to using only the freshest ingredients and its dedication to creating a warm and welcoming atmosphere for guests. I am excited about the opportunity to be a part of a team that shares my passion for delivering exceptional customer experiences.
-In addition to my technical skills and experience, I possess a strong work ethic and a willingness to learn and adapt to new situations. I am available to work a variety of shifts, including weekends and holidays, and I am committed to providing outstanding service to every guest, every time.
-Thank you for considering my application. I would be thrilled to discuss this opportunity further and explain in greater detail why I am the ideal candidate for this role. Please do not hesitate to contact me at [Your Phone Number] or [Your Email Address].
-Sincerely,
-[Your Name]</t>
+          <t>Internship Application</t>
         </is>
       </c>
       <c r="K3" s="7" t="inlineStr">
+        <is>
+          <t>I am excited to apply for the Waiter position at Cattleman's Ranch, and I am confident that my skills and enthusiasm make me an ideal candidate for the role. As a 20-year-old with a strong passion for delivering exceptional customer service, I am eager to join your team and contribute to providing an outstanding dining experience for your guests. With a friendly and approachable demeanor, I am well-suited to work in a fast-paced environment and ensure that every customer leaves with a positive impression.
+I would welcome the opportunity to discuss my application and how I can contribute to the success of Cattleman's Ranch. Please feel free to contact me to arrange an interview at your convenience. I have attached my resume for your review, and I look forward to the opportunity to meet with you to discuss how my skills and experience align with the needs of your team. Thank you for considering my application. Sincerely, Nakul</t>
+        </is>
+      </c>
+      <c r="L3" s="7" t="inlineStr">
         <is>
           <t>Email Sent.</t>
         </is>
@@ -633,7 +629,7 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2</v>
@@ -648,31 +644,21 @@
       </c>
       <c r="I4" s="7" t="inlineStr">
         <is>
-          <t>For the position of salesman at TupperWare</t>
+          <t>Write an cover letter for sending and email to TupperWare's HR, Ms Arianne Jane. I want to work as a salesman there. Make it short and concise, just 2 paragraphs. My name is Nakul and 20 years old. No need to add subject line and NO PREAMBLE!</t>
         </is>
       </c>
       <c r="J4" s="7" t="inlineStr">
         <is>
-          <t>[Your Name]
-[Your Address]
-[City, State, ZIP]
-[Date]
-[Hiring Manager's Name]
-TupperWare
-[TupperWare's Address]
-[City, State, ZIP]
-Dear [Hiring Manager's Name],
-I am excited to apply for the Salesman position at TupperWare, a renowned brand that has been a household name for decades. With a passion for building relationships and driving sales growth, I am confident that my skills and experience make me an ideal fit for this role.
-As a highly motivated and results-driven sales professional, I have a proven track record of consistently meeting and exceeding sales targets. My excellent communication and interpersonal skills enable me to effectively engage with customers, understand their needs, and provide tailored solutions that meet their expectations. I am well-versed in product knowledge and have a keen ability to demonstrate the benefits and features of TupperWare's innovative products.
-I am particularly drawn to TupperWare's commitment to providing high-quality, durable, and functional products that make a positive impact on people's lives. I am impressed by the company's dedication to empowering individuals, especially women, through its business opportunities and community involvement. As someone who values integrity, teamwork, and customer satisfaction, I am excited about the opportunity to join an organization that shares these values.
-In my current role at [Current Company], I have gained valuable experience in sales, customer service, and team management. I have successfully developed and executed sales strategies, built strong relationships with customers, and consistently achieved sales targets. I am confident that my skills and experience will enable me to make a significant contribution to TupperWare's sales team.
-I am excited about the opportunity to work with TupperWare's iconic products and to be part of a team that is dedicated to making a positive impact on people's lives. I am confident that my passion, energy, and sales expertise make me an ideal candidate for this role. I would welcome the opportunity to discuss my application and how I can contribute to TupperWare's success.
-Thank you for considering my application. I look forward to the opportunity to meet with you to discuss this role further.
-Sincerely,
-[Your Name]</t>
+          <t>Internship Application</t>
         </is>
       </c>
       <c r="K4" s="7" t="inlineStr">
+        <is>
+          <t>I am excited to apply for the Salesman position at TupperWare, and I am confident that my skills and enthusiasm make me an ideal candidate for the role. At 20 years old, I possess a strong passion for sales and a drive to succeed in a fast-paced and dynamic environment. I am impressed by TupperWare's commitment to providing high-quality products and exceptional customer service, and I am eager to be a part of a team that shares my values.
+I would welcome the opportunity to discuss my application and how I can contribute to the success of TupperWare. I have attached my resume for your review, and I look forward to the opportunity to meet with you to discuss my qualifications further. Thank you for considering my application. I can be reached at your convenience to schedule an interview. Sincerely, Nakul</t>
+        </is>
+      </c>
+      <c r="L4" s="7" t="inlineStr">
         <is>
           <t>Email Sent.</t>
         </is>

</xml_diff>